<commit_message>
Modified pCT experimental file naming file
After 07/25/15 run, some changes were made to the way files will be
named during the scan, although the naming scheme used did not conform
to the format established prior to the run.  These are minor changes
made in an attempt to come closer to the naming scheme that was used at
the time of the run which is clearly what feels more natural when
creating them.  These are minor changes.
</commit_message>
<xml_diff>
--- a/Phantoms/pCT_Phantom_List.xlsx
+++ b/Phantoms/pCT_Phantom_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="7380"/>
+    <workbookView xWindow="240" yWindow="2355" windowWidth="14805" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,21 +157,6 @@
     <t>LinePair</t>
   </si>
   <si>
-    <t>_4</t>
-  </si>
-  <si>
-    <t>_3</t>
-  </si>
-  <si>
-    <t>_2</t>
-  </si>
-  <si>
-    <t>_1</t>
-  </si>
-  <si>
-    <t>_0</t>
-  </si>
-  <si>
     <t>Continuous Scan Tag</t>
   </si>
   <si>
@@ -292,21 +277,6 @@
     <t>Emp_XXXX_000.dat</t>
   </si>
   <si>
-    <t>Calib_XXXX_0_000.dat</t>
-  </si>
-  <si>
-    <t>Calib_XXXX_1_000.dat</t>
-  </si>
-  <si>
-    <t>Calib_XXXX_2_000.dat</t>
-  </si>
-  <si>
-    <t>Calib_XXXX_3_000.dat</t>
-  </si>
-  <si>
-    <t>Calib_XXXX_4_000.dat</t>
-  </si>
-  <si>
     <t>CIRSEdge_XXXX_xxx.dat</t>
   </si>
   <si>
@@ -409,10 +379,40 @@
     <t>nosteps 4 bricks</t>
   </si>
   <si>
-    <t>_nst4</t>
-  </si>
-  <si>
-    <t>Calib_XXXX_nst4_000.dat</t>
+    <t>_0b</t>
+  </si>
+  <si>
+    <t>_1b</t>
+  </si>
+  <si>
+    <t>_2b</t>
+  </si>
+  <si>
+    <t>_3b</t>
+  </si>
+  <si>
+    <t>_4b</t>
+  </si>
+  <si>
+    <t>_nst4b</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_4b_000.dat</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_3b_000.dat</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_2b_000.dat</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_1b_000.dat</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_0b_000.dat</t>
+  </si>
+  <si>
+    <t>Calib_XXXX_nst4b_000.dat</t>
   </si>
 </sst>
 </file>
@@ -1128,6 +1128,12 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1164,14 +1170,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,7 +1484,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,21 +1507,21 @@
       <c r="A1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="70">
+      <c r="B1" s="72">
         <v>42210</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69"/>
+      <c r="B2" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -1530,82 +1530,82 @@
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="73"/>
+        <v>73</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="75"/>
       <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="74"/>
+        <v>74</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="76"/>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="66"/>
+        <v>74</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="68"/>
       <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="66" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="66"/>
+        <v>74</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="68"/>
       <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="66"/>
+      <c r="D8" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="68"/>
       <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1617,36 +1617,36 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="28" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>8</v>
@@ -1661,24 +1661,24 @@
         <v>29</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="46"/>
       <c r="I11" s="23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J11" s="53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K11" s="46"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>21</v>
@@ -1687,181 +1687,181 @@
         <v>20</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G12" s="47"/>
       <c r="H12" s="46"/>
       <c r="I12" s="23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J12" s="53" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K12" s="46"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="65" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="76" t="s">
-        <v>54</v>
+      <c r="E13" s="77" t="s">
+        <v>49</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G13" s="49" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="39" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J13" s="54" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="K13" s="46"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="76"/>
+      <c r="E14" s="77"/>
       <c r="F14" s="36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="H14" s="46"/>
       <c r="I14" s="25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J14" s="55" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="76"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="H15" s="46"/>
       <c r="I15" s="25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="77"/>
       <c r="F16" s="36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G16" s="52" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="H16" s="46"/>
       <c r="I16" s="25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="K16" s="46"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="77"/>
       <c r="F17" s="44" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G17" s="57" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="H17" s="46"/>
       <c r="I17" s="25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="K17" s="46"/>
     </row>
     <row r="18" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="77"/>
       <c r="F18" s="44" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G18" s="49" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H18" s="46"/>
       <c r="I18" s="24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J18" s="56" t="s">
         <v>132</v>
@@ -1883,20 +1883,20 @@
         <v>4</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1914,20 +1914,20 @@
         <v>3</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J20" s="58" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K20" s="58" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1945,20 +1945,20 @@
         <v>32</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G21" s="47"/>
       <c r="H21" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J21" s="58" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K21" s="58" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1976,20 +1976,20 @@
         <v>31</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G22" s="47"/>
       <c r="H22" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J22" s="58" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K22" s="58" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2007,27 +2007,27 @@
         <v>33</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G23" s="47"/>
       <c r="H23" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J23" s="58" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K23" s="58" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="63" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -2036,243 +2036,243 @@
       <c r="D24" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="75" t="s">
+      <c r="E24" s="63" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="46"/>
       <c r="I24" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J24" s="59" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="K24" s="60"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="77"/>
-      <c r="B25" s="75"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="75"/>
+      <c r="E25" s="63"/>
       <c r="F25" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>36</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J25" s="61" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K25" s="62" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="63" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="75" t="s">
+      <c r="E26" s="63" t="s">
         <v>44</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>37</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J26" s="59" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K26" s="59" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="77"/>
-      <c r="B27" s="75"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="75"/>
+      <c r="E27" s="63"/>
       <c r="F27" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J27" s="61" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K27" s="61" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="75" t="s">
+      <c r="E28" s="63" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>37</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J28" s="59" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="K28" s="59" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="77"/>
-      <c r="B29" s="75"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="75"/>
+      <c r="E29" s="63"/>
       <c r="F29" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J29" s="61" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="K29" s="61" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="63" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="75" t="s">
+      <c r="E30" s="63" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J30" s="59" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="K30" s="59" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="77"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="75"/>
+      <c r="E31" s="63"/>
       <c r="F31" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J31" s="61" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="K31" s="61" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2280,7 +2280,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="14" t="s">
@@ -2290,20 +2290,20 @@
         <v>43</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J32" s="58" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K32" s="58" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2314,11 +2314,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E13:E18"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
@@ -2327,11 +2327,11 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A30:A31"/>

</xml_diff>

<commit_message>
pCT data format update
Continued modifications to reflect Kodiak storage directory moves and
expanded descriptions of data directories including relevant information
related to other developments
</commit_message>
<xml_diff>
--- a/Phantoms/pCT_Phantom_List.xlsx
+++ b/Phantoms/pCT_Phantom_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2355" windowWidth="14805" windowHeight="7380"/>
+    <workbookView xWindow="240" yWindow="2805" windowWidth="14805" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1131,8 +1131,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1170,8 +1170,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1482,15 +1482,15 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
@@ -1715,7 +1715,7 @@
       <c r="D13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="64" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="35" t="s">
@@ -1744,7 +1744,7 @@
       <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="77"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="36" t="s">
         <v>72</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="D15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="77"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="36" t="s">
         <v>72</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="77"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="36" t="s">
         <v>72</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="D17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="77"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="44" t="s">
         <v>72</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="D18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="77"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="44" t="s">
         <v>72</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="77" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="63" t="s">
@@ -2055,7 +2055,7 @@
       <c r="K24" s="60"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="63"/>
       <c r="C25" s="17" t="s">
         <v>16</v>
@@ -2084,7 +2084,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="77" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="63" t="s">
@@ -2119,7 +2119,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
+      <c r="A27" s="77"/>
       <c r="B27" s="63"/>
       <c r="C27" s="17" t="s">
         <v>53</v>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="77" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="63" t="s">
@@ -2183,7 +2183,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="63"/>
       <c r="C29" s="17" t="s">
         <v>53</v>
@@ -2212,7 +2212,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="77" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="63" t="s">
@@ -2247,7 +2247,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="63"/>
       <c r="C31" s="17" t="s">
         <v>55</v>
@@ -2314,11 +2314,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
@@ -2327,14 +2330,11 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E13:E18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>